<commit_message>
Implement custom Deserializer not to use string in API body param
</commit_message>
<xml_diff>
--- a/doc/API_doc.xlsx
+++ b/doc/API_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\liar\LiarGameServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66F1F05-0A08-4B66-8EFD-28ABADA22D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49122528-3EAF-40C6-BAEC-61834FDEA4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$K$36</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="214">
   <si>
     <t>단계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -441,43 +444,6 @@
     <t>*spring state machine 분석
 *chattingcontroller test 코드구현
 *gameContoller startGame test 코드 구현중</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>senderId:String
-message:{
-            "method":String
-            "body":JSON.stringify
-            (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>round:int,
-            category:list&lt;string&gt;,
-            turn:int</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-        },
-"uuid":String</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -577,10 +543,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>requestTurnFinish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>*Front 테스트 구현 및 버그 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -774,16 +736,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"startRound", "body":{}}, "uuid":"7d9fd1d0-078d-443b-85cd-249b2ac021f2"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>senderId:String
-message:{
-            "method":String
-            "body":JSON.stringify
-            (</t>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
     </r>
     <r>
       <rPr>
@@ -795,7 +749,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>state:String</t>
+      <t>notifyLiarSelected</t>
     </r>
     <r>
       <rPr>
@@ -806,19 +760,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)
-        },
-"uuid":String</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>senderId:String
-message:{
-            "method":String
-            "body":JSON.stringify
-            (</t>
+      <t>", "body":{</t>
     </r>
     <r>
       <rPr>
@@ -830,7 +772,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"{}"</t>
+      <t>"liar":true/false</t>
     </r>
     <r>
       <rPr>
@@ -841,17 +783,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)
-        },
-"uuid":String</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"SERVER", "message":
-{"method":"notifyRoundStarted", "body":
-JSON.stringify({</t>
+      <t>,</t>
     </r>
     <r>
       <rPr>
@@ -863,7 +795,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"state":"SELECT_LIAR","round":int</t>
+      <t>"state":"OPEN_KEYWORD"</t>
     </r>
     <r>
       <rPr>
@@ -874,141 +806,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>})
-}, "uuid":String}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>openKeyword</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":"6c9bfe42-4a37-4ede-a7a8-76ecd80c958a"}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"SERVER", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>notifyLiarSelected</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"liar":true/false</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"state":"OPEN_KEYWORD"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>}}, "uuid":'dcd4e79d-8908-4e3c-968b-b5b9addccf16'}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>selectLiar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":"dcd4e79d-8908-4e3c-968b-b5b9addccf16"}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1175,35 +973,6 @@
   </si>
   <si>
     <r>
-      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>requestTurnFinished</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":"f8542777-28de-4a11-ab30-ed45ba4bf762"}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"voteLiar", "body":{</t>
     </r>
     <r>
@@ -1282,39 +1051,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>}, "uuid":'02c2fccd-f151-462f-b41b-b233da62cd22'}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"senderId":String, "message":{"method":"openLiar", "body":{}}, "uuid":String}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"2f76478e-163c-4df5-a158-de39f02c9fef", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>openLiar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":'a97103ee-f9d6-429f-9723-35486b4e3731'}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1495,94 +1231,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>{"senderId":"SERVER", "message":
-{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>notifyTurnTimeout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":"8044cf67-0083-4fa4-acbd-ef40788a6057"}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"SERVER", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>notifyLiarAnswerNeeded</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":"89e48c7e-fbb2-4b94-b9ae-022890deff7f"}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerNeeded", "body":</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>}, "uuid":String}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{"senderId":"String, "message":{"method":"checkKeywordCorrect", 
 "body":{"keyword":String}}, "uuid":String}</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1660,41 +1308,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"senderId":String, "message":{"method":"openScore", "body":{}}, 
-"uuid":String}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{"senderId":"SERVER", "message":{"method":"notifyScores", "body":{"scoreBoard":Map&lt;String,int&gt;}}, "uuid":String}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"85b753c2-90cf-4522-a7af-d900b41b2711", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>openScore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":"59d33d69-5270-44ec-9d94-4ede767a5161"}</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1797,12 +1411,6 @@
   </si>
   <si>
     <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerCorrect", "body":{"answer":boolean,"state":"PUBLISH_SCORE"}}, "uuid":String}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*타임아웃관련 API
-*라운드처리
-*랭킹 처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1906,40 +1514,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"senderId":String, "message":{"method":"publishRankings", "body":{}}, 
-"uuid":String}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"b8dc11a0-9717-4146-9e8d-650812da4adc", "message":{"method":"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>publishRankings</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "body":{}}, "uuid":"a291045e-f3b1-4572-8564-109601340261"}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>{"senderId":"SERVER", "message":{"method":"</t>
     </r>
@@ -2108,21 +1682,41 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"senderId":"SERVER", "message":{"method":"notifyVoteTimeout", "body":{}}, "uuid":'e10a1066-7497-4fa5-bae5-82145746bdfa'}</t>
-  </si>
-  <si>
-    <t>{"senderId":"SERVER", "message":{"method":"notifyVoteTimeout", "body":{}}, "uuid":String}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*테스트코드 리팩토링
+    <t>/subscribe/system/private/{userId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*API message body 파라미터 jsonSubtype 사용해서 변경-&gt;body를 string으로 감싸지 않아도됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JWT
+예외처리 앱으로 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*테스트코드 리팩토링(ConcurrentLinkedQueue vs LinkedBlockingQueue)
 *timeout 구현 및 테스트코드 작성
 *랭킹 처리 구현 및 테스트코드 작성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    <t>*API message body 파라미터 jsonSubtype 사용해서 변경했을때 
+파라미터로 type같은것을 추가로 넣어야함
+그러지 않기위해 JsonTypeInfo.Id.DEDUCTION로 변경했으나 문제 있었음
+deserializer를 직접구현하여 해결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requestTurnFinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>senderId:String
+message:{
+            "method":String
+            "body":{</t>
     </r>
     <r>
       <rPr>
@@ -2134,7 +1728,9 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>notifyLiarAnswerTimeOut</t>
+      <t>round:int,
+            category:list&lt;string&gt;,
+            turn:int}</t>
     </r>
     <r>
       <rPr>
@@ -2145,13 +1741,48 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>", "body":{}}, "uuid":String}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>{"senderId":"SERVER", "message":{"method":"</t>
+      <t xml:space="preserve">
+        },
+"uuid":String</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>senderId:String
+message:{
+            "method":String
+            "body":
+            ("{}")
+        },
+"uuid":String</t>
+  </si>
+  <si>
+    <t>senderId:String
+message:{
+            "method":String
+            "body":{state:String}
+        },
+"uuid":String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":
+{"method":"notifyRoundStarted", "body":
+{"state":"SELECT_LIAR","round":int}
+}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>senderId:String
+message:{
+            "method":String
+        },
+"uuid":String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"</t>
     </r>
     <r>
       <rPr>
@@ -2163,7 +1794,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>notifyLiarAnswerTimeOut</t>
+      <t>selectLiar</t>
     </r>
     <r>
       <rPr>
@@ -2174,9 +1805,98 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>", "body":{}}, "uuid":"1d27327f-30dd-4b1c-92b0-a6105392c211"}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+      <t>"}, "uuid":"dcd4e79d-8908-4e3c-968b-b5b9addccf16"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*테스트코드 deserializer 도입하면서 fail되는 부분들 해결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타이머 개선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state machine 도입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":
+{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyTurnTimeout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":null}, "uuid":"8044cf67-0083-4fa4-acbd-ef40788a6057"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"startRound", "body":null}, "uuid":"7d9fd1d0-078d-443b-85cd-249b2ac021f2"}</t>
+  </si>
+  <si>
+    <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"openKeyword", "body":null}, "uuid":"6c9bfe42-4a37-4ede-a7a8-76ecd80c958a"}</t>
+  </si>
+  <si>
+    <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"requestTurnFinished", "body":null}, "uuid":"f8542777-28de-4a11-ab30-ed45ba4bf762"}</t>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyVoteTimeout", "body":null}, "uuid":String}</t>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyVoteTimeout", "body":null}, "uuid":'e10a1066-7497-4fa5-bae5-82145746bdfa'}</t>
+  </si>
+  <si>
+    <t>{"senderId":String, "message":{"method":"openLiar", "body":null}, "uuid":String}</t>
+  </si>
+  <si>
+    <t>{"senderId":"2f76478e-163c-4df5-a158-de39f02c9fef", "message":{"method":"openLiar", "body":null}, "uuid":'a97103ee-f9d6-429f-9723-35486b4e3731'}</t>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerNeeded", "body":null}, "uuid":String}</t>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerNeeded", "body":null}, "uuid":"89e48c7e-fbb2-4b94-b9ae-022890deff7f"}</t>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerTimeOut", "body":null}, "uuid":String}</t>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerTimeOut", "body":null}, "uuid":"1d27327f-30dd-4b1c-92b0-a6105392c211"}</t>
+  </si>
+  <si>
+    <t>{"senderId":String, "message":{"method":"openScore", "body":null}, 
+"uuid":String}</t>
+  </si>
+  <si>
+    <t>{"senderId":"85b753c2-90cf-4522-a7af-d900b41b2711", "message":{"method":"openScore", "body":null}, "uuid":"59d33d69-5270-44ec-9d94-4ede767a5161"}</t>
+  </si>
+  <si>
+    <t>{"senderId":String, "message":{"method":"publishRankings", "body":null}, 
+"uuid":String}</t>
+  </si>
+  <si>
+    <t>{"senderId":"b8dc11a0-9717-4146-9e8d-650812da4adc", "message":{"method":"publishRankings", "body":null}, "uuid":"a291045e-f3b1-4572-8564-109601340261"}</t>
   </si>
 </sst>
 </file>
@@ -2664,8 +2384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2690,7 +2410,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -2705,7 +2425,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2731,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>49</v>
@@ -2766,7 +2486,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="132" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -2783,21 +2503,21 @@
         <v>4</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="99" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
@@ -2812,19 +2532,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>67</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>138</v>
+        <v>191</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>57</v>
@@ -2943,16 +2663,16 @@
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>54</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -2972,23 +2692,23 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>68</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -3005,16 +2725,16 @@
         <v>4</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>55</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>139</v>
+        <v>193</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -3034,19 +2754,19 @@
         <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>69</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>56</v>
@@ -3060,7 +2780,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3</v>
@@ -3069,16 +2789,16 @@
         <v>4</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -3086,7 +2806,7 @@
     <row r="16" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>44</v>
@@ -3098,19 +2818,19 @@
         <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K16" s="7"/>
     </row>
@@ -3131,16 +2851,16 @@
         <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>80</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>158</v>
+        <v>198</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -3151,7 +2871,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>4</v>
@@ -3160,16 +2880,16 @@
         <v>11</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>71</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>81</v>
@@ -3184,7 +2904,7 @@
         <v>77</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>62</v>
@@ -3193,16 +2913,16 @@
         <v>4</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>109</v>
+        <v>188</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>147</v>
+        <v>201</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -3220,19 +2940,19 @@
         <v>11</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K20" s="7"/>
     </row>
@@ -3253,16 +2973,16 @@
         <v>4</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>59</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -3282,19 +3002,19 @@
         <v>11</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>82</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>65</v>
@@ -3315,16 +3035,16 @@
         <v>11</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>83</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
@@ -3343,15 +3063,17 @@
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="G24" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H24" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>202</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
@@ -3371,16 +3093,16 @@
         <v>4</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>66</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>150</v>
+        <v>204</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
@@ -3400,16 +3122,16 @@
         <v>11</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>84</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>92</v>
@@ -3418,13 +3140,13 @@
     </row>
     <row r="27" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>4</v>
@@ -3433,16 +3155,16 @@
         <v>33</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>93</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
@@ -3453,7 +3175,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>33</v>
@@ -3462,16 +3184,16 @@
         <v>4</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>95</v>
@@ -3493,16 +3215,16 @@
         <v>11</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>94</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
@@ -3513,7 +3235,7 @@
         <v>36</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>4</v>
@@ -3522,16 +3244,16 @@
         <v>11</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>96</v>
@@ -3546,7 +3268,7 @@
         <v>38</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>3</v>
@@ -3555,16 +3277,16 @@
         <v>4</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
@@ -3572,7 +3294,7 @@
     <row r="32" spans="1:11" ht="132" x14ac:dyDescent="0.3">
       <c r="A32" s="15"/>
       <c r="B32" s="5" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>37</v>
@@ -3584,16 +3306,16 @@
         <v>11</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>97</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
@@ -3603,10 +3325,10 @@
         <v>46</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>4</v>
@@ -3615,29 +3337,29 @@
         <v>11</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>75</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>3</v>
@@ -3646,16 +3368,16 @@
         <v>4</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
@@ -3663,10 +3385,10 @@
     <row r="35" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>4</v>
@@ -3675,16 +3397,16 @@
         <v>11</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
@@ -3693,7 +3415,7 @@
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="7" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>4</v>
@@ -3702,21 +3424,22 @@
         <v>11</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:K36" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
   <mergeCells count="9">
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A30"/>
@@ -3735,17 +3458,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0688698-043E-4F34-83E0-0B082EC495A7}">
-  <dimension ref="B1:F12"/>
+  <dimension ref="B1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.25" customWidth="1"/>
-    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
@@ -3753,18 +3476,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B2" s="3">
         <v>44898</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3774,13 +3497,19 @@
       <c r="C3" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="F3" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>44900</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -3788,7 +3517,7 @@
         <v>44902</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3796,7 +3525,7 @@
         <v>44906</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -3804,7 +3533,7 @@
         <v>44908</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -3812,7 +3541,7 @@
         <v>44909</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3820,7 +3549,7 @@
         <v>44913</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3828,7 +3557,7 @@
         <v>44914</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3836,7 +3565,7 @@
         <v>44918</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3844,7 +3573,31 @@
         <v>44919</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>204</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>44924</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>44926</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>44927</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new API for notify room owner to open liar
</commit_message>
<xml_diff>
--- a/doc/API_doc.xlsx
+++ b/doc/API_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\liar\LiarGameServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AEE616-5B25-43A3-93A6-C1AB1DA185B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F539D065-8D74-43FB-8D53-9461E754A3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$K$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$K$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="221">
   <si>
     <t>단계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,10 +139,6 @@
   </si>
   <si>
     <t>투표결과리턴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5-1-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1904,6 +1900,33 @@
     <t>*Exception handler 도입 및 TC추가
 *일부 TC 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5-1-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이어공개 요청하라고 알림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/subscribe/system/private/{roomId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notifyLiarOpenRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarOpenRequest", "body":null}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarOpenRequest", "body":GameStateResponse(state=OPEN_LIAR)}, "uuid":'2ba42775-2afc-4fe0-b6ad-d7e86db4229b'}</t>
   </si>
 </sst>
 </file>
@@ -2389,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2417,7 +2440,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -2432,7 +2455,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2443,7 +2466,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -2458,16 +2481,16 @@
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>7</v>
@@ -2478,10 +2501,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="4"/>
@@ -2495,7 +2518,7 @@
     </row>
     <row r="5" spans="1:11" ht="132" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -2510,16 +2533,16 @@
         <v>4</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -2539,44 +2562,44 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -2585,10 +2608,10 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>4</v>
@@ -2598,10 +2621,10 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -2610,21 +2633,21 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -2633,7 +2656,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
@@ -2644,10 +2667,10 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -2655,13 +2678,13 @@
     </row>
     <row r="11" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -2670,16 +2693,16 @@
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -2699,25 +2722,25 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>16</v>
@@ -2732,16 +2755,16 @@
         <v>4</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -2761,33 +2784,33 @@
         <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3</v>
@@ -2796,16 +2819,16 @@
         <v>4</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -2813,10 +2836,10 @@
     <row r="16" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>4</v>
@@ -2825,31 +2848,31 @@
         <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>4</v>
@@ -2858,16 +2881,16 @@
         <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -2878,7 +2901,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>4</v>
@@ -2887,49 +2910,49 @@
         <v>11</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -2938,7 +2961,7 @@
       <c r="A20" s="15"/>
       <c r="B20" s="5"/>
       <c r="C20" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>4</v>
@@ -2947,25 +2970,25 @@
         <v>11</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G20" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="J20" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>21</v>
@@ -2980,16 +3003,16 @@
         <v>4</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -3009,31 +3032,31 @@
         <v>11</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="99" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>4</v>
@@ -3042,16 +3065,16 @@
         <v>11</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
@@ -3059,10 +3082,10 @@
     <row r="24" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>4</v>
@@ -3071,50 +3094,50 @@
         <v>11</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H24" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>200</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="99" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="5" t="s">
-        <v>28</v>
+        <v>215</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>30</v>
+        <v>216</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="F25" s="4" t="s">
-        <v>131</v>
+        <v>217</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>66</v>
+        <v>218</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="132" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="5" t="s">
         <v>27</v>
@@ -3123,126 +3146,126 @@
         <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>128</v>
-      </c>
+    <row r="27" spans="1:11" ht="132" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>152</v>
+        <v>28</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="J27" s="7"/>
+        <v>140</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+    <row r="28" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>127</v>
+      </c>
       <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>146</v>
+        <v>202</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>95</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" ht="99" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
       <c r="B29" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>34</v>
+        <v>157</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G29" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="99" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
       <c r="B30" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>4</v>
@@ -3251,91 +3274,89 @@
         <v>11</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>205</v>
+        <v>159</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>96</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>47</v>
-      </c>
+      <c r="A31" s="15"/>
       <c r="B31" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>113</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H31" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-    </row>
-    <row r="32" spans="1:11" ht="132" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>46</v>
-      </c>
+    <row r="33" spans="1:11" ht="132" x14ac:dyDescent="0.3">
+      <c r="A33" s="15"/>
       <c r="B33" s="5" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>4</v>
@@ -3344,85 +3365,89 @@
         <v>11</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="99" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>164</v>
+        <v>45</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>113</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>167</v>
+        <v>74</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>210</v>
+        <v>172</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+    <row r="35" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="B35" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>176</v>
+        <v>208</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="C36" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>4</v>
@@ -3431,29 +3456,56 @@
         <v>11</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
+    <row r="37" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A3:K36" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
+  <autoFilter ref="A3:K37" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
   <mergeCells count="9">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A21:A25"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
@@ -3480,7 +3532,7 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3488,13 +3540,13 @@
         <v>44898</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3502,10 +3554,10 @@
         <v>44899</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -3513,10 +3565,10 @@
         <v>44900</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -3524,7 +3576,7 @@
         <v>44902</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3532,7 +3584,7 @@
         <v>44906</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -3540,7 +3592,7 @@
         <v>44908</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -3548,7 +3600,7 @@
         <v>44909</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3556,7 +3608,7 @@
         <v>44913</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3564,7 +3616,7 @@
         <v>44914</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3572,7 +3624,7 @@
         <v>44918</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3580,7 +3632,7 @@
         <v>44919</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3588,7 +3640,7 @@
         <v>44924</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="66" x14ac:dyDescent="0.3">
@@ -3596,7 +3648,7 @@
         <v>44926</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -3604,7 +3656,7 @@
         <v>44927</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="66" x14ac:dyDescent="0.3">
@@ -3612,7 +3664,7 @@
         <v>44928</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="33" x14ac:dyDescent="0.3">
@@ -3620,7 +3672,7 @@
         <v>44934</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify message mapping prefix Add exception handler case
</commit_message>
<xml_diff>
--- a/doc/API_doc.xlsx
+++ b/doc/API_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\liar\LiarGameServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F539D065-8D74-43FB-8D53-9461E754A3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3164A500-5E1F-4070-9448-487A32114943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="224">
   <si>
     <t>단계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -509,32 +509,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/publish/system/private/{roomId}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 또는 /publish/system/public/{roomId}/API</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -632,16 +606,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/publish/system/private/{roomId}</t>
-  </si>
-  <si>
-    <t>/subscribe/system/public/{roomId}</t>
-  </si>
-  <si>
-    <t>/subscribe/system/public/{roomId}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>턴 종료요청</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -716,10 +680,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/publish/system/private/{roomId}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"startGame", "body":{"round":5,"turn":2,"category":["food","sports"]}}, "uuid":"a8f5bdc9-3cc7-4d9f-bde5-71ef471b9308"}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1289,10 +1249,6 @@
   </si>
   <si>
     <t>openScores</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/subscribe/system/private/{liarId}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1671,10 +1627,6 @@
       </rPr>
       <t>}}, "uuid":String}</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/subscribe/system/private/{userId}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1914,10 +1866,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/subscribe/system/private/{roomId}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>notifyLiarOpenRequest</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1927,6 +1875,44 @@
   </si>
   <si>
     <t>{"senderId":"SERVER", "message":{"method":"notifyLiarOpenRequest", "body":GameStateResponse(state=OPEN_LIAR)}, "uuid":'2ba42775-2afc-4fe0-b6ad-d7e86db4229b'}</t>
+  </si>
+  <si>
+    <t>/publish/private/{roomId} 또는 /publish/public/{roomId}/API</t>
+  </si>
+  <si>
+    <t>/publish/private/{roomId}</t>
+  </si>
+  <si>
+    <t>/subscribe/public/{roomId}</t>
+  </si>
+  <si>
+    <t>/subscribe/private/{userId}</t>
+  </si>
+  <si>
+    <t>/subscribe/private/{roomId}</t>
+  </si>
+  <si>
+    <t>/subscribe/private/{liarId}</t>
+  </si>
+  <si>
+    <t>에러발생시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요청한클라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":String?, "body":{ErrorResult:String}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/subscribe/errors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*message mapping prefix 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2016,7 +2002,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2039,6 +2025,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2048,7 +2047,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2096,6 +2095,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2412,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2440,7 +2454,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -2455,7 +2469,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="8" t="s">
-        <v>105</v>
+        <v>213</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2481,7 +2495,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>48</v>
@@ -2533,16 +2547,16 @@
         <v>4</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>49</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -2562,19 +2576,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>66</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>56</v>
@@ -2693,16 +2707,16 @@
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>53</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -2722,19 +2736,19 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>67</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K12" s="7"/>
     </row>
@@ -2755,16 +2769,16 @@
         <v>4</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>112</v>
+        <v>214</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>54</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -2784,19 +2798,19 @@
         <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>68</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>55</v>
@@ -2819,16 +2833,16 @@
         <v>4</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>112</v>
+        <v>214</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>102</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -2836,7 +2850,7 @@
     <row r="16" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>43</v>
@@ -2848,7 +2862,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>69</v>
@@ -2857,10 +2871,10 @@
         <v>104</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K16" s="7"/>
     </row>
@@ -2881,16 +2895,16 @@
         <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H17" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>187</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>194</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -2901,7 +2915,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>4</v>
@@ -2910,16 +2924,16 @@
         <v>11</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>80</v>
@@ -2934,7 +2948,7 @@
         <v>76</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>61</v>
@@ -2943,16 +2957,16 @@
         <v>4</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -2970,19 +2984,19 @@
         <v>11</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K20" s="7"/>
     </row>
@@ -3003,16 +3017,16 @@
         <v>4</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>58</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -3032,19 +3046,19 @@
         <v>11</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>81</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>64</v>
@@ -3065,16 +3079,16 @@
         <v>11</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>82</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
@@ -3082,7 +3096,7 @@
     <row r="24" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="5" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>77</v>
@@ -3094,16 +3108,16 @@
         <v>11</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>78</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
@@ -3111,10 +3125,10 @@
     <row r="25" spans="1:11" ht="99" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="5" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>4</v>
@@ -3126,13 +3140,13 @@
         <v>217</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
@@ -3152,16 +3166,16 @@
         <v>4</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>65</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
@@ -3181,16 +3195,16 @@
         <v>11</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>83</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>91</v>
@@ -3199,13 +3213,13 @@
     </row>
     <row r="28" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>4</v>
@@ -3214,16 +3228,16 @@
         <v>32</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>150</v>
+        <v>218</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>92</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
@@ -3234,7 +3248,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>32</v>
@@ -3243,16 +3257,16 @@
         <v>4</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>94</v>
@@ -3274,16 +3288,16 @@
         <v>11</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>93</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
@@ -3294,7 +3308,7 @@
         <v>35</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>4</v>
@@ -3303,16 +3317,16 @@
         <v>11</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>95</v>
@@ -3327,7 +3341,7 @@
         <v>37</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>3</v>
@@ -3336,16 +3350,16 @@
         <v>4</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>112</v>
+        <v>214</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
@@ -3353,7 +3367,7 @@
     <row r="33" spans="1:11" ht="132" x14ac:dyDescent="0.3">
       <c r="A33" s="15"/>
       <c r="B33" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>36</v>
@@ -3365,16 +3379,16 @@
         <v>11</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>96</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
@@ -3384,10 +3398,10 @@
         <v>45</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>4</v>
@@ -3396,29 +3410,29 @@
         <v>11</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>74</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
     <row r="35" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>3</v>
@@ -3427,16 +3441,16 @@
         <v>4</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>112</v>
+        <v>214</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
@@ -3444,10 +3458,10 @@
     <row r="36" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>4</v>
@@ -3456,46 +3470,67 @@
         <v>11</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="7" t="s">
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="H37" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="I37" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+    </row>
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B38" s="5"/>
+      <c r="C38" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D38" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
+      <c r="E38" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:K37" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
@@ -3517,10 +3552,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0688698-043E-4F34-83E0-0B082EC495A7}">
-  <dimension ref="B1:F17"/>
+  <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3543,10 +3578,10 @@
         <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3557,7 +3592,7 @@
         <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -3568,7 +3603,7 @@
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -3576,7 +3611,7 @@
         <v>44902</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3584,7 +3619,7 @@
         <v>44906</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -3592,7 +3627,7 @@
         <v>44908</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -3600,7 +3635,7 @@
         <v>44909</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3608,7 +3643,7 @@
         <v>44913</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3616,7 +3651,7 @@
         <v>44914</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3624,7 +3659,7 @@
         <v>44918</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3632,7 +3667,7 @@
         <v>44919</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3640,7 +3675,7 @@
         <v>44924</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="66" x14ac:dyDescent="0.3">
@@ -3648,7 +3683,7 @@
         <v>44926</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -3656,7 +3691,7 @@
         <v>44927</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="66" x14ac:dyDescent="0.3">
@@ -3664,7 +3699,7 @@
         <v>44928</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="33" x14ac:dyDescent="0.3">
@@ -3672,7 +3707,15 @@
         <v>44934</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>44935</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add getGameCategory API request and response Add category and keywords
</commit_message>
<xml_diff>
--- a/doc/API_doc.xlsx
+++ b/doc/API_doc.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\liar\LiarGameServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3164A500-5E1F-4070-9448-487A32114943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3608B91C-CC12-49E8-BA16-F61B71D66C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$K$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="222">
   <si>
     <t>단계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,18 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>할일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameManager</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RoundController</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -261,14 +249,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>랜덤한 한 사람 추출하여 전달</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임정보 저장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>라운드 시작 요청</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -297,10 +277,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>투표결과 과반수넘었는지 확인하기.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>openLiar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -329,10 +305,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>턴 순서에 따라 이번턴에 누구인지 말해줌. 턴 타임아웃 스레드 돌리기. 그에 따라 GameManager에 턴타임아웃이라고 말해주기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>턴타임아웃 알림</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -361,10 +333,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.타임아웃 안끝났으면 끝내기 1.RoundController에게 이번턴에 누구인지 알려달라고 요청. 2. 턴알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>notifyVoteResult</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -405,23 +373,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>현재 state 확인. RoundController에게 말해서 라이어 공개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>notifyLiarAnswerNeeded</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>notifyLiarAnswerCorrect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>현재 state확인. 요청자가 라이어가 맞는지확인. RoundController에게 정답여부 요청. check_liar_answer state로 변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RoundController에 점수계산요청</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -611,42 +567,6 @@
   </si>
   <si>
     <t>현재 턴 알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.현재 state 확인
-1. RoundController에게 라이어투표 결과리턴. 
-2.과반수를 넘었으면 state 변경(OPEN_LIAR로)
-3.과반수를 못넘겼으면 state(VOTE_LIAR 그대로)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. RoundController에게 카테고리 및 키워드 요청. 
-2.카테고리 및 키워드 알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.현재 state 확인 
-1. RoundController에게 라이어선정 요청. 
-2.라이어정보 알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0. 정확한 round인지 확인 
-1.현재 state확인하여, status 변경(BEFORE_ROUND-&gt;SELECT_LIAR) 
-2.알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. RoundController에게 게임정보 전달 
-2.현재 state확인하여, status 변경(BEFORE_START-&gt;BEFORE_ROUND) 
-3.알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">마지막턴확인해서, 해당 이벤트날려줌
-0. VOTE_LIAR state 변경. vote 타임아웃설정
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1912,6 +1832,66 @@
   </si>
   <si>
     <t>*message mapping prefix 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*카테고리 얻어오는 API 추가
+*WSS 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/subscribe/private/{ownerId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리 답장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:{"senderId":"SERVER", "message":{"method":"notifyGameCategory", "body":GameCategoryResponse(category=[celebrity, sports, food])}, "uuid":'07676428-f80f-4470-89a5-5175ab2562e5'}</t>
+  </si>
+  <si>
+    <t>getGameCategory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notifyGameCategory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:{"senderId":"SERVER", "message":{"method":"notifyGameCategory", "body":"category"={String})}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":String, "message":{"method":"getGameCategory", "body":null}, 
+"uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"4fa45167-0905-4ba4-be72-dca928be6852", "message":{"method":"getGameCategory", "body":null}, "uuid":'07676428-f80f-4470-89a5-5175ab2562e5'}</t>
+  </si>
+  <si>
+    <t>현재 게임 상태 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 상태 알림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getGameState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notifyGameState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>END_GAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2002,7 +1982,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2038,6 +2018,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2047,12 +2053,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2064,9 +2067,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2096,19 +2096,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2426,1115 +2456,1112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.875" customWidth="1"/>
-    <col min="8" max="8" width="36" style="2" customWidth="1"/>
-    <col min="9" max="9" width="33.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="40.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="3"/>
+    <col min="5" max="5" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="36" style="5" customWidth="1"/>
+    <col min="9" max="9" width="33.625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="6" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="132" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="8" t="s">
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" ht="99" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" ht="99" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" ht="132" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:10" ht="99" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="C20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="1:10" ht="231" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:10" ht="99" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10" ht="99" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="1:10" ht="132" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J29" s="16"/>
+    </row>
+    <row r="30" spans="1:10" ht="99" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J30" s="16"/>
+    </row>
+    <row r="31" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="J31" s="16"/>
+    </row>
+    <row r="32" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="1:10" ht="132" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:10" ht="99" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="27"/>
+      <c r="B36" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="28"/>
+      <c r="C38" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="C39" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J39" s="16"/>
+    </row>
+    <row r="40" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="C40" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G40" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" ht="132" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="H40" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="F41" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C42" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="1:11" ht="132" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" ht="231" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="5" t="s">
+      <c r="E42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="1:11" ht="132" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K31" s="7"/>
-    </row>
-    <row r="32" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-    </row>
-    <row r="33" spans="1:11" ht="132" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-    </row>
-    <row r="34" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-    </row>
-    <row r="35" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-    </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B38" s="5"/>
-      <c r="C38" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="20" t="s">
+      <c r="G42" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:K37" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
-  <mergeCells count="9">
+  <autoFilter ref="A3:I37" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
+  <mergeCells count="10">
+    <mergeCell ref="A35:A36"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3552,10 +3579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0688698-043E-4F34-83E0-0B082EC495A7}">
-  <dimension ref="B1:F18"/>
+  <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3567,155 +3594,163 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>44898</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>101</v>
+      <c r="C2" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>205</v>
+        <v>133</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>44899</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>99</v>
+      <c r="C3" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>44900</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>44902</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>44906</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>44908</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>44909</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>44913</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>44914</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>44918</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>44919</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <v>44924</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>44926</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <v>44927</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>44928</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
-        <v>44902</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
-        <v>44906</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="3">
-        <v>44908</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
-        <v>44909</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B9" s="3">
-        <v>44913</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
-        <v>44914</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
-        <v>44918</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
-        <v>44919</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <v>44924</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <v>44926</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
-        <v>44927</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
-        <v>44928</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
     <row r="17" spans="2:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>44934</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>44935</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="3">
-        <v>44935</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>223</v>
+    <row r="19" spans="2:3" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <v>44936</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introduce JWT -Fix timer cancel -Modify Room service API -Introduce room.login,room.logout
</commit_message>
<xml_diff>
--- a/doc/API_doc.xlsx
+++ b/doc/API_doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\liar\LiarGameServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3608B91C-CC12-49E8-BA16-F61B71D66C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C07A3DF-DEED-43F5-9BF5-F321B40C46E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>라이어선정 요청</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -362,14 +358,6 @@
   </si>
   <si>
     <t>1-3-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>notifyMemberLeft</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>notifyMemberEntered</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1809,9 +1797,6 @@
     <t>/subscribe/private/{userId}</t>
   </si>
   <si>
-    <t>/subscribe/private/{roomId}</t>
-  </si>
-  <si>
     <t>/subscribe/private/{liarId}</t>
   </si>
   <si>
@@ -1892,6 +1877,22 @@
   </si>
   <si>
     <t>END_GAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/subscribe/private/{userId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이어 선택 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/subscribe/room/{roomId}/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/subscribe/room/{roomId}/logout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2053,7 +2054,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2093,15 +2094,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2114,32 +2106,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2448,7 +2434,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2458,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2477,36 +2463,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="16"/>
+      <c r="A1"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="16"/>
+      <c r="A2"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="1"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -2521,31 +2507,31 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" s="16"/>
+        <v>83</v>
+      </c>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="16"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>36</v>
+      <c r="A5" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -2560,21 +2546,21 @@
         <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="J5" s="16"/>
+        <v>106</v>
+      </c>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2588,48 +2574,48 @@
         <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J6" s="16"/>
+        <v>107</v>
+      </c>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="16"/>
+        <v>77</v>
+      </c>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>4</v>
@@ -2637,37 +2623,37 @@
       <c r="E8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>82</v>
+      <c r="F8" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>4</v>
@@ -2675,23 +2661,23 @@
       <c r="E10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>81</v>
+      <c r="F10" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J10" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>38</v>
+      <c r="A11" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>3</v>
@@ -2700,21 +2686,21 @@
         <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="J11" s="16"/>
+        <v>168</v>
+      </c>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
@@ -2728,28 +2714,28 @@
         <v>8</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="J12" s="16"/>
+        <v>109</v>
+      </c>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>39</v>
+      <c r="A13" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>14</v>
+        <v>219</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>3</v>
@@ -2758,26 +2744,26 @@
         <v>4</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="J13" s="16"/>
+        <v>164</v>
+      </c>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>4</v>
@@ -2786,28 +2772,28 @@
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J14" s="16"/>
+        <v>108</v>
+      </c>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>41</v>
+      <c r="A15" s="21" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>3</v>
@@ -2816,26 +2802,26 @@
         <v>4</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>4</v>
@@ -2844,28 +2830,28 @@
         <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="J16" s="16"/>
+        <v>111</v>
+      </c>
+      <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>37</v>
+      <c r="A17" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>4</v>
@@ -2874,26 +2860,26 @@
         <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="J17" s="16"/>
+        <v>167</v>
+      </c>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>4</v>
@@ -2902,51 +2888,51 @@
         <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="J18" s="16"/>
+        <v>110</v>
+      </c>
+      <c r="J18" s="13"/>
     </row>
     <row r="19" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J19" s="16"/>
+        <v>170</v>
+      </c>
+      <c r="J19" s="13"/>
     </row>
     <row r="20" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="21"/>
       <c r="C20" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>4</v>
@@ -2955,28 +2941,28 @@
         <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="J20" s="16"/>
+        <v>153</v>
+      </c>
+      <c r="J20" s="13"/>
     </row>
     <row r="21" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
-        <v>44</v>
+      <c r="A21" s="21" t="s">
+        <v>43</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -2985,26 +2971,26 @@
         <v>4</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="J21" s="16"/>
+        <v>112</v>
+      </c>
+      <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:10" ht="231" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>4</v>
@@ -3013,26 +2999,26 @@
         <v>8</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J22" s="16"/>
+        <v>113</v>
+      </c>
+      <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>4</v>
@@ -3041,26 +3027,26 @@
         <v>8</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="J23" s="16"/>
+        <v>118</v>
+      </c>
+      <c r="J23" s="13"/>
     </row>
     <row r="24" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>4</v>
@@ -3069,26 +3055,26 @@
         <v>8</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="J24" s="16"/>
+        <v>172</v>
+      </c>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
@@ -3097,26 +3083,26 @@
         <v>3</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="J25" s="16"/>
+        <v>192</v>
+      </c>
+      <c r="J25" s="13"/>
     </row>
     <row r="26" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>3</v>
@@ -3125,26 +3111,26 @@
         <v>4</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="J26" s="16"/>
+        <v>174</v>
+      </c>
+      <c r="J26" s="13"/>
     </row>
     <row r="27" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
@@ -3153,84 +3139,84 @@
         <v>8</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J27" s="16"/>
+        <v>115</v>
+      </c>
+      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>106</v>
+      <c r="A28" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="J28" s="16"/>
+        <v>176</v>
+      </c>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="J29" s="16"/>
+        <v>121</v>
+      </c>
+      <c r="J29" s="13"/>
     </row>
     <row r="30" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
@@ -3239,26 +3225,26 @@
         <v>8</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="J30" s="16"/>
+        <v>132</v>
+      </c>
+      <c r="J30" s="13"/>
     </row>
     <row r="31" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>4</v>
@@ -3267,28 +3253,28 @@
         <v>8</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="J31" s="16"/>
+        <v>178</v>
+      </c>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
-        <v>43</v>
+      <c r="A32" s="21" t="s">
+        <v>42</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>3</v>
@@ -3297,26 +3283,26 @@
         <v>4</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="J32" s="16"/>
+        <v>180</v>
+      </c>
+      <c r="J32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>4</v>
@@ -3325,28 +3311,28 @@
         <v>8</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J33" s="16"/>
+        <v>127</v>
+      </c>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="99" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>4</v>
@@ -3355,28 +3341,28 @@
         <v>8</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J34" s="16"/>
+        <v>147</v>
+      </c>
+      <c r="J34" s="13"/>
     </row>
     <row r="35" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="26" t="s">
-        <v>140</v>
+      <c r="A35" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>3</v>
@@ -3385,26 +3371,26 @@
         <v>4</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G35" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="23"/>
+      <c r="B36" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="J35" s="16"/>
-    </row>
-    <row r="36" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>4</v>
@@ -3413,25 +3399,25 @@
         <v>8</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="J36" s="16"/>
+        <v>149</v>
+      </c>
+      <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>4</v>
@@ -3440,126 +3426,126 @@
         <v>8</v>
       </c>
       <c r="F37" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
+      <c r="C38" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="J37" s="16"/>
-    </row>
-    <row r="38" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="C38" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="J38" s="16"/>
+        <v>200</v>
+      </c>
+      <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
       <c r="C39" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G39" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J39" s="16"/>
+      <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
       <c r="C40" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H40" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="I40" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="J40" s="13"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G41" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+        <v>194</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C42" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:I37" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
+  <autoFilter ref="A3:I42" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}"/>
   <mergeCells count="10">
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="A26:A27"/>
@@ -3594,7 +3580,7 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3602,13 +3588,13 @@
         <v>44898</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3616,10 +3602,10 @@
         <v>44899</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -3627,10 +3613,10 @@
         <v>44900</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -3638,7 +3624,7 @@
         <v>44902</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3646,7 +3632,7 @@
         <v>44906</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -3654,7 +3640,7 @@
         <v>44908</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -3662,7 +3648,7 @@
         <v>44909</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3670,7 +3656,7 @@
         <v>44913</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3678,7 +3664,7 @@
         <v>44914</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3686,7 +3672,7 @@
         <v>44918</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -3694,7 +3680,7 @@
         <v>44919</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -3702,7 +3688,7 @@
         <v>44924</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="66" x14ac:dyDescent="0.3">
@@ -3710,7 +3696,7 @@
         <v>44926</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -3718,7 +3704,7 @@
         <v>44927</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="66" x14ac:dyDescent="0.3">
@@ -3726,7 +3712,7 @@
         <v>44928</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="33" x14ac:dyDescent="0.3">
@@ -3734,7 +3720,7 @@
         <v>44934</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
@@ -3742,15 +3728,15 @@
         <v>44935</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="33" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>44936</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>207</v>
+      <c r="C19" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>